<commit_message>
update to spreadsheet cleaning
</commit_message>
<xml_diff>
--- a/Data/top_50_frat_email.xlsx
+++ b/Data/top_50_frat_email.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/michaeltopper/Desktop/Fraternities and Sexual Assault/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76291A66-AA06-FE43-9A77-224C78D6E4CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A91BAA61-3581-574C-AC86-2F42C5391A10}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1440" yWindow="2680" windowWidth="28920" windowHeight="19720" xr2:uid="{0FD14FDD-C3E9-104A-A17A-FCA1DA63B27B}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="73">
   <si>
     <t>university</t>
   </si>
@@ -250,13 +250,16 @@
   </si>
   <si>
     <t>no 2019 or december 2018</t>
+  </si>
+  <si>
+    <t>was this included?</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -274,6 +277,14 @@
       <u/>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -296,15 +307,18 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -619,8 +633,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D23E8EE9-0FA6-3946-A13B-C7F5BBF2087F}">
   <dimension ref="A1:H51"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="183" zoomScaleNormal="183" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView tabSelected="1" topLeftCell="A24" zoomScale="183" zoomScaleNormal="183" workbookViewId="0">
+      <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1019,6 +1033,9 @@
       <c r="D23">
         <v>1</v>
       </c>
+      <c r="E23">
+        <v>1</v>
+      </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
@@ -1095,6 +1112,9 @@
       <c r="D28">
         <v>1</v>
       </c>
+      <c r="E28">
+        <v>1</v>
+      </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
@@ -1118,9 +1138,9 @@
         <v>31</v>
       </c>
       <c r="D30">
-        <v>0</v>
-      </c>
-      <c r="G30" t="s">
+        <v>1</v>
+      </c>
+      <c r="G30" s="3" t="s">
         <v>61</v>
       </c>
     </row>
@@ -1252,6 +1272,9 @@
       <c r="D39">
         <v>1</v>
       </c>
+      <c r="E39">
+        <v>1</v>
+      </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
@@ -1398,6 +1421,9 @@
       <c r="D49">
         <v>1</v>
       </c>
+      <c r="E49">
+        <v>1</v>
+      </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
@@ -1429,8 +1455,17 @@
       <c r="D51">
         <v>1</v>
       </c>
+      <c r="E51">
+        <v>1</v>
+      </c>
+      <c r="G51" t="s">
+        <v>72</v>
+      </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="G30" r:id="rId1" xr:uid="{86931273-B410-EE46-9417-80A8B7D5FC7C}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
compare clery and dcl graphs
</commit_message>
<xml_diff>
--- a/Data/top_50_frat_email.xlsx
+++ b/Data/top_50_frat_email.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/michaeltopper/Desktop/Fraternities and Sexual Assault/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D90894AB-9F39-464E-9E0F-FF6463717DD3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8873ECD7-01CC-5848-B925-F72D43377FCB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="37100" yWindow="500" windowWidth="28920" windowHeight="19720" xr2:uid="{0FD14FDD-C3E9-104A-A17A-FCA1DA63B27B}"/>
+    <workbookView xWindow="2200" yWindow="1280" windowWidth="28920" windowHeight="19720" xr2:uid="{0FD14FDD-C3E9-104A-A17A-FCA1DA63B27B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -189,9 +189,6 @@
     <t>obtained</t>
   </si>
   <si>
-    <t>include</t>
-  </si>
-  <si>
     <t>notes</t>
   </si>
   <si>
@@ -210,9 +207,6 @@
     <t>looks like I can webscrape if needed. Might be a pain</t>
   </si>
   <si>
-    <t>referred me to the websight</t>
-  </si>
-  <si>
     <t>cleaned</t>
   </si>
   <si>
@@ -250,6 +244,12 @@
   </si>
   <si>
     <t>The University of Alabama</t>
+  </si>
+  <si>
+    <t>moratorium</t>
+  </si>
+  <si>
+    <t>included</t>
   </si>
 </sst>
 </file>
@@ -637,8 +637,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D23E8EE9-0FA6-3946-A13B-C7F5BBF2087F}">
   <dimension ref="A1:H51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A33" zoomScale="183" zoomScaleNormal="183" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="183" zoomScaleNormal="183" workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -647,7 +647,7 @@
     <col min="2" max="2" width="17.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -661,18 +661,21 @@
         <v>50</v>
       </c>
       <c r="E1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="F1" t="s">
+        <v>71</v>
+      </c>
+      <c r="G1" t="s">
         <v>51</v>
       </c>
-      <c r="G1" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -686,10 +689,16 @@
       <c r="E2">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="F2">
+        <v>1</v>
+      </c>
+      <c r="H2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B3">
         <v>2</v>
@@ -703,11 +712,17 @@
       <c r="E3">
         <v>0</v>
       </c>
+      <c r="F3">
+        <v>0</v>
+      </c>
       <c r="G3" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+        <v>62</v>
+      </c>
+      <c r="H3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -723,11 +738,17 @@
       <c r="E4">
         <v>1</v>
       </c>
+      <c r="F4">
+        <v>1</v>
+      </c>
       <c r="G4" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+        <v>60</v>
+      </c>
+      <c r="H4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -747,10 +768,13 @@
         <v>0</v>
       </c>
       <c r="G5" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+        <v>52</v>
+      </c>
+      <c r="H5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -766,13 +790,19 @@
       <c r="E6">
         <v>1</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" ht="18" x14ac:dyDescent="0.2">
+      <c r="F6">
+        <v>1</v>
+      </c>
+      <c r="H6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D7">
         <v>0</v>
@@ -780,8 +810,11 @@
       <c r="E7">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -798,10 +831,13 @@
         <v>0</v>
       </c>
       <c r="G8" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+        <v>53</v>
+      </c>
+      <c r="H8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -817,8 +853,14 @@
       <c r="E9">
         <v>1</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="F9">
+        <v>1</v>
+      </c>
+      <c r="H9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>9</v>
       </c>
@@ -831,8 +873,11 @@
       <c r="E10">
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>10</v>
       </c>
@@ -848,8 +893,11 @@
       <c r="E11">
         <v>1</v>
       </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>11</v>
       </c>
@@ -862,8 +910,11 @@
       <c r="E12">
         <v>0</v>
       </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>12</v>
       </c>
@@ -880,10 +931,13 @@
         <v>1</v>
       </c>
       <c r="G13" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+        <v>59</v>
+      </c>
+      <c r="H13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>13</v>
       </c>
@@ -896,8 +950,11 @@
       <c r="E14">
         <v>0</v>
       </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>14</v>
       </c>
@@ -913,8 +970,11 @@
       <c r="E15">
         <v>1</v>
       </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>15</v>
       </c>
@@ -928,6 +988,9 @@
         <v>1</v>
       </c>
       <c r="E16">
+        <v>1</v>
+      </c>
+      <c r="H16">
         <v>1</v>
       </c>
     </row>
@@ -948,10 +1011,10 @@
         <v>1</v>
       </c>
       <c r="G17" t="s">
-        <v>57</v>
-      </c>
-      <c r="H17" t="s">
-        <v>58</v>
+        <v>56</v>
+      </c>
+      <c r="H17">
+        <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.2">
@@ -971,7 +1034,10 @@
         <v>0</v>
       </c>
       <c r="G18" t="s">
-        <v>65</v>
+        <v>63</v>
+      </c>
+      <c r="H18">
+        <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.2">
@@ -990,6 +1056,9 @@
       <c r="E19">
         <v>1</v>
       </c>
+      <c r="H19">
+        <v>1</v>
+      </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
@@ -1008,7 +1077,10 @@
         <v>1</v>
       </c>
       <c r="G20" s="2" t="s">
-        <v>66</v>
+        <v>64</v>
+      </c>
+      <c r="H20">
+        <v>0</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.2">
@@ -1027,6 +1099,9 @@
       <c r="E21">
         <v>1</v>
       </c>
+      <c r="H21">
+        <v>0</v>
+      </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
@@ -1044,6 +1119,9 @@
       <c r="E22">
         <v>1</v>
       </c>
+      <c r="H22">
+        <v>1</v>
+      </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
@@ -1061,6 +1139,9 @@
       <c r="E23">
         <v>1</v>
       </c>
+      <c r="H23">
+        <v>0</v>
+      </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
@@ -1078,6 +1159,9 @@
       <c r="E24">
         <v>1</v>
       </c>
+      <c r="H24">
+        <v>1</v>
+      </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
@@ -1095,6 +1179,9 @@
       <c r="E25">
         <v>1</v>
       </c>
+      <c r="H25">
+        <v>0</v>
+      </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
@@ -1109,6 +1196,9 @@
       <c r="E26">
         <v>0</v>
       </c>
+      <c r="H26">
+        <v>0</v>
+      </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
@@ -1126,6 +1216,9 @@
       <c r="E27">
         <v>1</v>
       </c>
+      <c r="H27">
+        <v>1</v>
+      </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
@@ -1143,6 +1236,9 @@
       <c r="E28">
         <v>1</v>
       </c>
+      <c r="H28">
+        <v>0</v>
+      </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
@@ -1160,6 +1256,9 @@
       <c r="E29">
         <v>1</v>
       </c>
+      <c r="H29">
+        <v>1</v>
+      </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A30" s="4" t="s">
@@ -1172,7 +1271,10 @@
         <v>1</v>
       </c>
       <c r="G30" s="3" t="s">
-        <v>68</v>
+        <v>66</v>
+      </c>
+      <c r="H30">
+        <v>0</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.2">
@@ -1191,6 +1293,9 @@
       <c r="E31">
         <v>1</v>
       </c>
+      <c r="H31">
+        <v>1</v>
+      </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
@@ -1208,8 +1313,11 @@
       <c r="E32">
         <v>1</v>
       </c>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H32">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>32</v>
       </c>
@@ -1225,8 +1333,11 @@
       <c r="E33">
         <v>1</v>
       </c>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H33">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>33</v>
       </c>
@@ -1239,8 +1350,11 @@
       <c r="E34">
         <v>0</v>
       </c>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H34">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>34</v>
       </c>
@@ -1257,10 +1371,13 @@
         <v>1</v>
       </c>
       <c r="G35" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
+        <v>66</v>
+      </c>
+      <c r="H35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>35</v>
       </c>
@@ -1270,8 +1387,11 @@
       <c r="E36">
         <v>0</v>
       </c>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H36">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>36</v>
       </c>
@@ -1287,8 +1407,11 @@
       <c r="E37">
         <v>1</v>
       </c>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H37">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>37</v>
       </c>
@@ -1301,8 +1424,11 @@
       <c r="E38">
         <v>0</v>
       </c>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>38</v>
       </c>
@@ -1318,8 +1444,11 @@
       <c r="E39">
         <v>1</v>
       </c>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H39">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>39</v>
       </c>
@@ -1336,10 +1465,13 @@
         <v>0</v>
       </c>
       <c r="G40" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
+        <v>61</v>
+      </c>
+      <c r="H40">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>40</v>
       </c>
@@ -1349,8 +1481,11 @@
       <c r="E41">
         <v>0</v>
       </c>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H41">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>41</v>
       </c>
@@ -1363,8 +1498,11 @@
       <c r="E42">
         <v>0</v>
       </c>
-    </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H42">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>42</v>
       </c>
@@ -1381,10 +1519,13 @@
         <v>0</v>
       </c>
       <c r="G43" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.2">
+        <v>67</v>
+      </c>
+      <c r="H43">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>43</v>
       </c>
@@ -1400,8 +1541,11 @@
       <c r="E44">
         <v>1</v>
       </c>
-    </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>44</v>
       </c>
@@ -1417,8 +1561,11 @@
       <c r="E45">
         <v>1</v>
       </c>
-    </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H45">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>45</v>
       </c>
@@ -1431,8 +1578,11 @@
       <c r="E46">
         <v>0</v>
       </c>
-    </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H46">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>46</v>
       </c>
@@ -1448,10 +1598,13 @@
       <c r="E47">
         <v>1</v>
       </c>
-    </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H47">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B48">
         <v>1</v>
@@ -1465,8 +1618,11 @@
       <c r="E48">
         <v>1</v>
       </c>
-    </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H48">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>47</v>
       </c>
@@ -1482,8 +1638,11 @@
       <c r="E49">
         <v>1</v>
       </c>
-    </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H49">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>48</v>
       </c>
@@ -1500,10 +1659,13 @@
         <v>1</v>
       </c>
       <c r="G50" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.2">
+        <v>54</v>
+      </c>
+      <c r="H50">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>49</v>
       </c>
@@ -1520,7 +1682,10 @@
         <v>1</v>
       </c>
       <c r="G51" t="s">
-        <v>67</v>
+        <v>65</v>
+      </c>
+      <c r="H51">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>